<commit_message>
project details with UI chnages
</commit_message>
<xml_diff>
--- a/MergeAttributesApplication/ProjectDetailsReport.xlsx
+++ b/MergeAttributesApplication/ProjectDetailsReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\Conti_AM\MergeAttributesApplication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E55D9C-CEBC-4691-A474-55D1CEC99B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BF1BE9-FBDF-46E4-89CE-CC9547A491BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="378">
   <si>
     <t>Project Name</t>
   </si>
@@ -1534,14 +1534,14 @@
   <dimension ref="A1:F178"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D182" sqref="D182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.54296875" customWidth="1"/>
+    <col min="3" max="3" width="53.54296875" customWidth="1"/>
     <col min="4" max="4" width="41" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
@@ -1685,6 +1685,9 @@
       <c r="C8" t="s">
         <v>24</v>
       </c>
+      <c r="D8" t="s">
+        <v>376</v>
+      </c>
       <c r="E8" t="s">
         <v>22</v>
       </c>
@@ -2298,7 +2301,7 @@
         <v>96</v>
       </c>
       <c r="D44" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="E44" t="s">
         <v>22</v>
@@ -4592,6 +4595,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F178" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="D2:D178" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Yes,No"</formula1>

</xml_diff>